<commit_message>
Fix the &%#$ branch status
</commit_message>
<xml_diff>
--- a/spreadsheets/Tasker_endpoints.xlsx
+++ b/spreadsheets/Tasker_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pknipp/Dropbox/AppAcad/weeks/TaskRabbitClone/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B018BDF9-EA2B-7C4A-A845-4524E8C441D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A590F8D-0E0B-CA49-A03D-55E25050A580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{3AD07EED-9D3A-6143-A75B-9D19FC2AFEFE}"/>
   </bookViews>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C00B5F-4350-EE4D-BB2C-AF3AB45FCCB3}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
@@ -692,17 +692,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="64" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="32" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <f>IF(A2="R","get",IF(A2="C","post",IF(A2="U","putch","delete")))</f>
-        <v>get</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <f>IF(B2="get","N","Y")</f>
-        <v>N</v>
+        <v>55</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -712,20 +710,19 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f>IF(B2="get","NA","yes")</f>
-        <v>NA</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="32" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -733,167 +730,158 @@
         <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4">
         <f>LEN(D3)-LEN(SUBSTITUTE(D3,"/",""))</f>
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>59</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <f>IF(A4="R","get",IF(A4="C","post",IF(A4="U","putch","delete")))</f>
-        <v>get</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <f>IF(B4="get","N","Y")</f>
-        <v>N</v>
+        <v>38</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4">
         <f>LEN(D4)-LEN(SUBSTITUTE(D4,"/",""))</f>
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f>IF(B4="get","NA","yes")</f>
-        <v>NA</v>
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E5" s="4">
         <f>LEN(D5)-LEN(SUBSTITUTE(D5,"/",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4" t="str">
         <f>IF(A6="R","get",IF(A6="C","post",IF(A6="U","putch","delete")))</f>
-        <v>post</v>
+        <v>delete</v>
       </c>
       <c r="C6" s="4" t="str">
         <f>IF(B6="get","N","Y")</f>
         <v>Y</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="E6" s="4">
         <f>LEN(D6)-LEN(SUBSTITUTE(D6,"/",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>13</v>
+        <v>68</v>
+      </c>
+      <c r="H6" s="1" t="str">
+        <f>IF(B6="get","NA","yes")</f>
+        <v>yes</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="B7" s="4" t="str">
+        <f>IF(A7="R","get",IF(A7="C","post",IF(A7="U","putch","delete")))</f>
+        <v>delete</v>
+      </c>
+      <c r="C7" s="4" t="str">
+        <f>IF(B7="get","N","Y")</f>
+        <v>Y</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4">
         <f>LEN(D7)-LEN(SUBSTITUTE(D7,"/",""))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8" s="4" t="str">
         <f>IF(A8="R","get",IF(A8="C","post",IF(A8="U","putch","delete")))</f>
-        <v>post</v>
+        <v>delete</v>
       </c>
       <c r="C8" s="4" t="str">
         <f>IF(B8="get","N","Y")</f>
         <v>Y</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E8" s="4">
         <f>LEN(D8)-LEN(SUBSTITUTE(D8,"/",""))</f>
@@ -902,11 +890,17 @@
       <c r="F8" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
@@ -919,63 +913,70 @@
         <v>N</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="E9" s="4">
         <f>LEN(D9)-LEN(SUBSTITUTE(D9,"/",""))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>62</v>
+        <v>6</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="H9" s="1" t="str">
         <f>IF(B9="get","NA","yes")</f>
         <v>NA</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="4" t="str">
         <f>IF(A10="R","get",IF(A10="C","post",IF(A10="U","putch","delete")))</f>
-        <v>putch</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>65</v>
+        <v>get</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <f>IF(B10="get","N","Y")</f>
+        <v>N</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="E10" s="4">
         <f>LEN(D10)-LEN(SUBSTITUTE(D10,"/",""))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="H10" s="1" t="str">
         <f>IF(B10="get","NA","yes")</f>
-        <v>yes</v>
+        <v>NA</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="str">
         <f>IF(A11="R","get",IF(A11="C","post",IF(A11="U","putch","delete")))</f>
-        <v>delete</v>
+        <v>get</v>
       </c>
       <c r="C11" s="4" t="str">
         <f>IF(B11="get","N","Y")</f>
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>49</v>
@@ -985,43 +986,50 @@
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>IF(B11="get","NA","yes")</f>
-        <v>yes</v>
+        <v>NA</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>IF(A12="R","get",IF(A12="C","post",IF(A12="U","putch","delete")))</f>
-        <v>post</v>
+        <v>get</v>
       </c>
       <c r="C12" s="4" t="str">
         <f>IF(B12="get","N","Y")</f>
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" s="4">
         <f>LEN(D12)-LEN(SUBSTITUTE(D12,"/",""))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f>IF(B12="get","NA","yes")</f>
+        <v>NA</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1057,93 +1065,91 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="64" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="str">
         <f>IF(A14="R","get",IF(A14="C","post",IF(A14="U","putch","delete")))</f>
-        <v>putch</v>
+        <v>get</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>IF(B14="get","N","Y")</f>
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E14" s="4">
         <f>LEN(D14)-LEN(SUBSTITUTE(D14,"/",""))</f>
-        <v>2</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H14" s="1" t="str">
+        <f>IF(B14="get","NA","yes")</f>
+        <v>NA</v>
+      </c>
       <c r="I14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="str">
         <f>IF(A15="R","get",IF(A15="C","post",IF(A15="U","putch","delete")))</f>
-        <v>delete</v>
+        <v>get</v>
       </c>
       <c r="C15" s="4" t="str">
         <f>IF(B15="get","N","Y")</f>
-        <v>Y</v>
+        <v>N</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" s="4">
         <f>LEN(D15)-LEN(SUBSTITUTE(D15,"/",""))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f>IF(B15="get","NA","yes")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <f>IF(A16="R","get",IF(A16="C","post",IF(A16="U","putch","delete")))</f>
-        <v>post</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="str" cm="1">
+        <f t="array" ref="B16">IF(A16="R","get",IF(B21A18="C","post",IF(A16="U","putch","delete")))</f>
+        <v>get</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <f>IF(B16="get","N","Y")</f>
+        <v>N</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E16" s="4">
         <f>LEN(D16)-LEN(SUBSTITUTE(D16,"/",""))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <f>IF(B16="get","NA","yes")</f>
+        <v>NA</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1181,32 +1187,35 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="str">
+        <f>IF(A18="R","get",IF(A18="C","post",IF(A18="U","putch","delete")))</f>
+        <v>get</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <f>IF(B18="get","N","Y")</f>
+        <v>N</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E18" s="4">
         <f>LEN(D18)-LEN(SUBSTITUTE(D18,"/",""))</f>
         <v>2</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f>IF(B18="get","NA","yes")</f>
+        <v>NA</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1222,67 +1231,65 @@
         <v>Y</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E19" s="4">
         <f>LEN(D19)-LEN(SUBSTITUTE(D19,"/",""))</f>
         <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" s="1" t="str">
-        <f>IF(B19="get","NA","yes")</f>
-        <v>yes</v>
+        <v>53</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20" s="4" t="str">
         <f>IF(A20="R","get",IF(A20="C","post",IF(A20="U","putch","delete")))</f>
-        <v>get</v>
+        <v>post</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>IF(B20="get","N","Y")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E20" s="4">
         <f>LEN(D20)-LEN(SUBSTITUTE(D20,"/",""))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="1" t="str">
-        <f>IF(B20="get","NA","yes")</f>
-        <v>NA</v>
+        <v>35</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4" t="str">
         <f>IF(A21="R","get",IF(A21="C","post",IF(A21="U","putch","delete")))</f>
-        <v>putch</v>
+        <v>post</v>
       </c>
       <c r="C21" s="4" t="str">
         <f>IF(B21="get","N","Y")</f>
         <v>Y</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E21" s="4">
         <f>LEN(D21)-LEN(SUBSTITUTE(D21,"/",""))</f>
@@ -1303,67 +1310,62 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="4" t="str">
         <f>IF(A22="R","get",IF(A22="C","post",IF(A22="U","putch","delete")))</f>
-        <v>delete</v>
+        <v>post</v>
       </c>
       <c r="C22" s="4" t="str">
         <f>IF(B22="get","N","Y")</f>
         <v>Y</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E22" s="4">
         <f>LEN(D22)-LEN(SUBSTITUTE(D22,"/",""))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="64" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="4" t="str">
         <f>IF(A23="R","get",IF(A23="C","post",IF(A23="U","putch","delete")))</f>
-        <v>get</v>
-      </c>
-      <c r="C23" s="4" t="str">
-        <f>IF(B23="get","N","Y")</f>
-        <v>N</v>
+        <v>post</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="4">
         <f>LEN(D23)-LEN(SUBSTITUTE(D23,"/",""))</f>
-        <v>3</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="1" t="str">
-        <f>IF(B23="get","NA","yes")</f>
-        <v>NA</v>
+        <v>10</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1379,112 +1381,110 @@
         <v>Y</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E24" s="4">
         <f>LEN(D24)-LEN(SUBSTITUTE(D24,"/",""))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f>IF(B24="get","NA","yes")</f>
+        <v>yes</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4" t="str">
         <f>IF(A25="R","get",IF(A25="C","post",IF(A25="U","putch","delete")))</f>
-        <v>get</v>
-      </c>
-      <c r="C25" s="4" t="str">
-        <f>IF(B25="get","N","Y")</f>
-        <v>N</v>
+        <v>putch</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E25" s="4">
         <f>LEN(D25)-LEN(SUBSTITUTE(D25,"/",""))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="H25" s="1" t="str">
         <f>IF(B25="get","NA","yes")</f>
-        <v>NA</v>
+        <v>yes</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B26" s="4" t="str">
         <f>IF(A26="R","get",IF(A26="C","post",IF(A26="U","putch","delete")))</f>
-        <v>get</v>
+        <v>putch</v>
       </c>
       <c r="C26" s="4" t="str">
         <f>IF(B26="get","N","Y")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E26" s="4">
         <f>LEN(D26)-LEN(SUBSTITUTE(D26,"/",""))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26" s="1" t="str">
-        <f>IF(B26="get","NA","yes")</f>
-        <v>NA</v>
+        <v>40</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="4" t="str" cm="1">
-        <f t="array" ref="B27">IF(A27="R","get",IF(B21A18="C","post",IF(A27="U","putch","delete")))</f>
-        <v>get</v>
+        <v>33</v>
+      </c>
+      <c r="B27" s="4" t="str">
+        <f>IF(A27="R","get",IF(A27="C","post",IF(A27="U","putch","delete")))</f>
+        <v>putch</v>
       </c>
       <c r="C27" s="4" t="str">
         <f>IF(B27="get","N","Y")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E27" s="4">
         <f>LEN(D27)-LEN(SUBSTITUTE(D27,"/",""))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="1" t="str">
-        <f>IF(B27="get","NA","yes")</f>
-        <v>NA</v>
+        <v>53</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J27">
-    <sortCondition ref="E2:E27"/>
+    <sortCondition ref="B2:B27"/>
     <sortCondition ref="D2:D27"/>
     <sortCondition ref="A2:A27" customList="C,R,U,D"/>
   </sortState>

</xml_diff>